<commit_message>
add references and data
</commit_message>
<xml_diff>
--- a/example/batch process paper section study.xlsx
+++ b/example/batch process paper section study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marct\AnacondaProjects\volume-em-pubs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\volume-em-pubs\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA9B162-DB5D-4B19-A848-0421BA92D9E9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDA9843-0A4A-4C98-9F80-8534F13B7CB3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="510" windowWidth="24255" windowHeight="15630" tabRatio="269" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="165" yWindow="1035" windowWidth="28245" windowHeight="12960" tabRatio="269" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="70">
   <si>
     <r>
       <t xml:space="preserve">Bock, D. D. </t>
@@ -341,9 +341,6 @@
   </si>
   <si>
     <t>microcircuitry of the cat retina - ?</t>
-  </si>
-  <si>
-    <t>Kasthuri S1 dense</t>
   </si>
   <si>
     <t>40 x 40</t>
@@ -965,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1482,7 +1479,7 @@
         <v>50</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>6</v>
@@ -1527,17 +1524,6 @@
       </c>
       <c r="J21" s="4" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H23" s="7">
-        <v>21</v>
-      </c>
-      <c r="I23" s="7">
-        <v>2015</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>